<commit_message>
updated results, wavelets ineffective
</commit_message>
<xml_diff>
--- a/CS 23X Project Experiments.xlsx
+++ b/CS 23X Project Experiments.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
-  <si>
-    <t>Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="72">
+  <si>
+    <t>Epoch Time</t>
   </si>
   <si>
     <t>Model Type</t>
@@ -49,7 +49,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>poop model</t>
+    <t>1s</t>
   </si>
   <si>
     <t>NN</t>
@@ -61,7 +61,7 @@
     <t>sca = .26</t>
   </si>
   <si>
-    <t>CNN1</t>
+    <t>50ms</t>
   </si>
   <si>
     <t>CNN</t>
@@ -143,6 +143,9 @@
     <t>dense(128,12)</t>
   </si>
   <si>
+    <t>4s</t>
+  </si>
+  <si>
     <t>CNN + FFT</t>
   </si>
   <si>
@@ -164,10 +167,7 @@
     <t>dropout 0  Epoch = 50</t>
   </si>
   <si>
-    <t>all with</t>
-  </si>
-  <si>
-    <t>same struc</t>
+    <t>same model</t>
   </si>
   <si>
     <t>dropout 0.1</t>
@@ -185,9 +185,6 @@
     <t>wt using db6 horizontal + vert (171x171x6) below</t>
   </si>
   <si>
-    <t>same business</t>
-  </si>
-  <si>
     <t xml:space="preserve">dropout 0 </t>
   </si>
   <si>
@@ -197,6 +194,9 @@
     <t>dropout .2</t>
   </si>
   <si>
+    <t>40s</t>
+  </si>
+  <si>
     <t>CNN2+WT</t>
   </si>
   <si>
@@ -209,20 +209,95 @@
     <t>(32conv3 drop max)x2</t>
   </si>
   <si>
-    <t>40s</t>
-  </si>
-  <si>
     <t>dropout .125</t>
   </si>
   <si>
     <t>dropout .175</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">DB6 </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> horiz Mean+ vert Mean + approx Mean (171x171x3) 
+epoch= 50</t>
+    </r>
+  </si>
+  <si>
+    <t>dropout  .2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>DB6</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> horiz Mean+ vert Mean + approx Mean (171x171x3) 
+Epoch = 100</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Roboto, RobotoDraft, Helvetica, Arial, sans-serif"/>
+        <b/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>HAAR</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Roboto, RobotoDraft, Helvetica, Arial, sans-serif"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> horiz Mean+ vert Mean + approx Mean (171x171x3)
+Epoch = 120</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Roboto, RobotoDraft, Helvetica, Arial, sans-serif"/>
+        <b/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>HAAR</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Roboto, RobotoDraft, Helvetica, Arial, sans-serif"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> horiz Mean+ vert Mean + approx Mean (171x171x3)
+Epoch = 120</t>
+    </r>
+  </si>
+  <si>
+    <t>** removed final dropout layer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -236,9 +311,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
     <font/>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +326,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor rgb="FF9FC5E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
   </fills>
@@ -258,15 +355,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -280,13 +377,38 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -525,28 +647,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -560,7 +682,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -583,7 +705,7 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -595,7 +717,7 @@
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="4"/>
@@ -608,20 +730,20 @@
     </row>
     <row r="4" ht="34.5" customHeight="1">
       <c r="A4" s="4"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="4"/>
@@ -631,19 +753,20 @@
       </c>
     </row>
     <row r="5" ht="34.5" customHeight="1">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>1.0E-7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="3">
+      <c r="F5" s="9"/>
+      <c r="G5" s="7">
         <v>0.147</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -682,16 +805,18 @@
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="7">
+      <c r="B8" s="9"/>
+      <c r="C8" s="8">
         <v>1.0E-6</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="7">
         <v>0.161</v>
       </c>
-      <c r="G8" s="3">
+      <c r="F8" s="9"/>
+      <c r="G8" s="7">
         <v>0.1766</v>
       </c>
     </row>
@@ -724,16 +849,18 @@
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="7">
+      <c r="B11" s="9"/>
+      <c r="C11" s="8">
         <v>1.0E-4</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="7">
         <v>0.213</v>
       </c>
-      <c r="G11" s="3">
+      <c r="F11" s="9"/>
+      <c r="G11" s="7">
         <v>0.208</v>
       </c>
     </row>
@@ -766,16 +893,18 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="7">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8">
         <v>0.01</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="7">
         <v>0.212</v>
       </c>
-      <c r="G14" s="3">
+      <c r="F14" s="9"/>
+      <c r="G14" s="7">
         <v>0.201</v>
       </c>
     </row>
@@ -808,28 +937,28 @@
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="7">
+      <c r="C17" s="8">
         <v>5.0E-5</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="7">
         <v>0.9963</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="7">
         <v>0.3277</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="7">
         <v>0.262</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="7">
         <v>0.0135</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="7">
         <v>2.3189</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="7">
         <v>5.1381</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -855,36 +984,39 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="7">
+        <v>43</v>
+      </c>
+      <c r="C18" s="8">
         <v>1.0E-7</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="D18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="7">
         <v>0.2167</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="7">
         <v>0.2156</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="7">
         <v>0.1766</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="7">
         <v>2.3409</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="7">
         <v>2.3522</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="7">
         <v>2.3461</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="7">
+      <c r="C19" s="10">
         <v>1.0E-7</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -910,11 +1042,11 @@
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="7">
+      <c r="C20" s="10">
         <v>1.0E-7</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" s="3">
         <v>0.2192</v>
@@ -936,11 +1068,11 @@
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="7">
+      <c r="C21" s="10">
         <v>1.0E-7</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E21" s="3">
         <v>0.1991</v>
@@ -962,33 +1094,33 @@
       </c>
     </row>
     <row r="22">
-      <c r="C22" s="7">
+      <c r="C22" s="8">
         <v>5.0E-6</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="D22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="7">
         <v>0.4076</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="7">
         <v>0.3615</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="7">
         <v>0.3967</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="7">
         <v>1.8374</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="7">
         <v>1.9143</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="7">
         <v>1.9367</v>
       </c>
     </row>
     <row r="23">
-      <c r="C23" s="7">
+      <c r="C23" s="10">
         <v>5.0E-6</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -1014,11 +1146,11 @@
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="7">
+      <c r="C24" s="10">
         <v>5.0E-6</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E24" s="3">
         <v>0.3608</v>
@@ -1040,11 +1172,11 @@
       </c>
     </row>
     <row r="25">
-      <c r="C25" s="7">
+      <c r="C25" s="10">
         <v>5.0E-6</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E25" s="3">
         <v>0.3748</v>
@@ -1066,33 +1198,33 @@
       </c>
     </row>
     <row r="26">
-      <c r="C26" s="7">
+      <c r="C26" s="8">
         <v>1.0E-5</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="D26" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="7">
         <v>0.4967</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="7">
         <v>0.3911</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="11">
         <v>0.4012</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="7">
         <v>1.541</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="7">
         <v>1.8728</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="7">
         <v>1.8897</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="7">
+      <c r="C27" s="10">
         <v>1.0E-5</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1118,11 +1250,11 @@
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="7">
+      <c r="C28" s="10">
         <v>1.0E-5</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E28" s="3">
         <v>0.4208</v>
@@ -1144,11 +1276,11 @@
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="7">
+      <c r="C29" s="10">
         <v>1.0E-5</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E29" s="3">
         <v>0.4121</v>
@@ -1170,33 +1302,33 @@
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="7">
+      <c r="C30" s="8">
         <v>5.0E-5</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="D30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="7">
         <v>0.9837</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="7">
         <v>0.3658</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="7">
         <v>0.3713</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="7">
         <v>0.2598</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="7">
         <v>2.3164</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="7">
         <v>2.183</v>
       </c>
     </row>
     <row r="31">
-      <c r="C31" s="7">
+      <c r="C31" s="10">
         <v>5.0E-5</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1222,11 +1354,11 @@
       </c>
     </row>
     <row r="32">
-      <c r="C32" s="7">
+      <c r="C32" s="10">
         <v>5.0E-5</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E32" s="3">
         <v>0.8041</v>
@@ -1248,11 +1380,11 @@
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="7">
+      <c r="C33" s="10">
         <v>5.0E-5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E33" s="3">
         <v>0.7354</v>
@@ -1274,33 +1406,33 @@
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="7">
+      <c r="C34" s="8">
         <v>1.0E-4</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="D34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="7">
         <v>0.9962</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="7">
         <v>0.3425</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="7">
         <v>0.3578</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="7">
         <v>0.1163</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="7">
         <v>2.718</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="7">
         <v>2.4789</v>
       </c>
     </row>
     <row r="35">
-      <c r="C35" s="7">
+      <c r="C35" s="10">
         <v>1.0E-4</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -1326,11 +1458,11 @@
       </c>
     </row>
     <row r="36">
-      <c r="C36" s="7">
+      <c r="C36" s="10">
         <v>1.0E-4</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E36" s="3">
         <v>0.8813</v>
@@ -1352,11 +1484,11 @@
       </c>
     </row>
     <row r="37">
-      <c r="C37" s="7">
+      <c r="C37" s="10">
         <v>1.0E-4</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E37" s="3">
         <v>0.8679</v>
@@ -1378,33 +1510,33 @@
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="7">
+      <c r="C38" s="8">
         <v>5.0E-4</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="3">
+      <c r="D38" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="7">
         <v>1.0</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="7">
         <v>0.334</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="7">
         <v>0.3323</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="7">
         <v>0.0013</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="7">
         <v>4.538</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="7">
         <v>4.3203</v>
       </c>
     </row>
     <row r="39">
-      <c r="C39" s="7">
+      <c r="C39" s="10">
         <v>5.0E-4</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -1430,11 +1562,11 @@
       </c>
     </row>
     <row r="40">
-      <c r="C40" s="7">
+      <c r="C40" s="10">
         <v>5.0E-4</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E40" s="3">
         <v>0.9944</v>
@@ -1456,11 +1588,11 @@
       </c>
     </row>
     <row r="41">
-      <c r="C41" s="7">
+      <c r="C41" s="10">
         <v>5.0E-4</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E41" s="3">
         <v>0.9875</v>
@@ -1482,33 +1614,33 @@
       </c>
     </row>
     <row r="42">
-      <c r="C42" s="7">
+      <c r="C42" s="8">
         <v>0.001</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E42" s="3">
+      <c r="D42" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="7">
         <v>1.0</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="7">
         <v>0.353</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="7">
         <v>0.3114</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42" s="8">
         <v>1.3158E-4</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="7">
         <v>5.1983</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="7">
         <v>5.5762</v>
       </c>
     </row>
     <row r="43">
-      <c r="C43" s="7">
+      <c r="C43" s="10">
         <v>0.001</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -1534,11 +1666,11 @@
       </c>
     </row>
     <row r="44">
-      <c r="C44" s="7">
+      <c r="C44" s="10">
         <v>0.001</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E44" s="3">
         <v>0.9952</v>
@@ -1560,11 +1692,11 @@
       </c>
     </row>
     <row r="45">
-      <c r="C45" s="7">
+      <c r="C45" s="10">
         <v>0.001</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E45" s="3">
         <v>0.9808</v>
@@ -1587,46 +1719,46 @@
     </row>
     <row r="46">
       <c r="D46" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B47" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="7">
+        <v>48</v>
+      </c>
+      <c r="C47" s="8">
         <v>5.0E-6</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E47" s="3">
+      <c r="D47" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="7">
         <v>0.336</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="7">
         <v>0.142</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="7">
         <v>0.133</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="7">
         <v>3.2</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="7">
         <v>5.6</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="7">
         <v>6.3</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M47" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="48">
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E48" s="3">
@@ -1649,7 +1781,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E49" s="3">
@@ -1672,7 +1804,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E50" s="3">
@@ -1695,33 +1827,33 @@
       </c>
     </row>
     <row r="51">
-      <c r="C51" s="7">
+      <c r="C51" s="8">
         <v>1.0E-5</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="3">
+      <c r="D51" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" s="7">
         <v>0.72</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="7">
         <v>0.163</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="7">
         <v>0.144</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="7">
         <v>0.96</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="7">
         <v>4.61</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="7">
         <v>4.73</v>
       </c>
     </row>
     <row r="52">
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E52" s="3">
@@ -1744,7 +1876,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E53" s="3">
@@ -1758,7 +1890,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E54" s="3">
@@ -1767,29 +1899,29 @@
       <c r="F54" s="3">
         <v>0.167</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="11">
         <v>0.2051</v>
       </c>
     </row>
     <row r="55">
-      <c r="C55" s="7">
+      <c r="C55" s="8">
         <v>5.0E-5</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E55" s="3">
+      <c r="D55" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" s="7">
         <v>1.0</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55" s="7">
         <v>0.144</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="7">
         <v>0.133</v>
       </c>
     </row>
     <row r="56">
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E56" s="3">
@@ -1803,7 +1935,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E57" s="3">
@@ -1817,7 +1949,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -1838,23 +1970,23 @@
         <v>55</v>
       </c>
       <c r="L59" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" s="8">
+        <v>5.0E-6</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60">
-      <c r="C60" s="7">
-        <v>5.0E-6</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E60" s="3">
+      <c r="E60" s="7">
         <v>0.3517</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60" s="7">
         <v>0.159</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="7">
         <v>0.1692</v>
       </c>
     </row>
@@ -1874,7 +2006,7 @@
     </row>
     <row r="62">
       <c r="D62" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E62" s="3">
         <v>0.2337</v>
@@ -1888,7 +2020,7 @@
     </row>
     <row r="63">
       <c r="D63" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E63" s="3">
         <v>0.1701</v>
@@ -1902,7 +2034,7 @@
     </row>
     <row r="64">
       <c r="D64" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E64" s="3">
         <v>0.1539</v>
@@ -1915,19 +2047,19 @@
       </c>
     </row>
     <row r="65">
-      <c r="C65" s="7">
+      <c r="C65" s="8">
         <v>1.0E-5</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E65" s="3">
+      <c r="D65" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="7">
         <v>0.7471</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="7">
         <v>0.167</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="7">
         <v>0.1557</v>
       </c>
     </row>
@@ -1947,7 +2079,7 @@
     </row>
     <row r="67">
       <c r="D67" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E67" s="3">
         <v>0.2496</v>
@@ -1961,7 +2093,7 @@
     </row>
     <row r="68">
       <c r="D68" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E68" s="3">
         <v>0.2308</v>
@@ -1975,7 +2107,7 @@
     </row>
     <row r="69">
       <c r="D69" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E69" s="3">
         <v>0.2069</v>
@@ -1988,19 +2120,19 @@
       </c>
     </row>
     <row r="70">
-      <c r="C70" s="7">
+      <c r="C70" s="8">
         <v>5.0E-5</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E70" s="3">
+      <c r="D70" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" s="7">
         <v>1.0</v>
       </c>
-      <c r="F70" s="3">
+      <c r="F70" s="7">
         <v>0.1438</v>
       </c>
-      <c r="G70" s="3">
+      <c r="G70" s="7">
         <v>0.1332</v>
       </c>
     </row>
@@ -2020,7 +2152,7 @@
     </row>
     <row r="72">
       <c r="D72" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E72" s="3">
         <v>0.4553</v>
@@ -2034,7 +2166,7 @@
     </row>
     <row r="73">
       <c r="D73" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E73" s="3">
         <v>0.3702</v>
@@ -2048,7 +2180,7 @@
     </row>
     <row r="74">
       <c r="D74" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E74" s="3">
         <v>0.281</v>
@@ -2056,11 +2188,14 @@
       <c r="F74" s="3">
         <v>0.2008</v>
       </c>
-      <c r="G74" s="3">
+      <c r="G74" s="11">
         <v>0.2096</v>
       </c>
     </row>
     <row r="75">
+      <c r="A75" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="B75" s="3" t="s">
         <v>60</v>
       </c>
@@ -2090,205 +2225,202 @@
       </c>
     </row>
     <row r="76">
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="8">
+        <v>1.0E-6</v>
+      </c>
+      <c r="D76" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C76" s="7">
-        <v>1.0E-6</v>
-      </c>
-      <c r="D76" s="3" t="s">
+      <c r="E76" s="7">
+        <v>0.1083</v>
+      </c>
+      <c r="F76" s="7">
+        <v>0.0803</v>
+      </c>
+      <c r="G76" s="7">
+        <v>0.0793</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="D77" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="3">
+        <v>0.1705</v>
+      </c>
+      <c r="F77" s="3">
+        <v>0.1649</v>
+      </c>
+      <c r="G77" s="3">
+        <v>0.1512</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="D78" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E76" s="3">
-        <v>0.1083</v>
-      </c>
-      <c r="F76" s="3">
-        <v>0.0803</v>
-      </c>
-      <c r="G76" s="3">
-        <v>0.0793</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="D77" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E77" s="9">
-        <v>0.1705</v>
-      </c>
-      <c r="F77" s="9">
+      <c r="E78" s="3">
+        <v>0.1457</v>
+      </c>
+      <c r="F78" s="3">
+        <v>0.1353</v>
+      </c>
+      <c r="G78" s="3">
+        <v>0.1437</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="D79" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0.0966</v>
+      </c>
+      <c r="F79" s="3">
+        <v>0.1205</v>
+      </c>
+      <c r="G79" s="3">
+        <v>0.1063</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="C80" s="8">
+        <v>5.0E-5</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0.1773</v>
+      </c>
+      <c r="F80" s="7">
+        <v>0.241</v>
+      </c>
+      <c r="G80" s="7">
+        <v>0.1766</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="D81" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E81" s="3">
+        <v>0.2103</v>
+      </c>
+      <c r="F81" s="3">
         <v>0.1649</v>
       </c>
-      <c r="G77" s="9">
-        <v>0.1512</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="D78" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E78" s="9">
-        <v>0.1457</v>
-      </c>
-      <c r="F78" s="9">
-        <v>0.1353</v>
-      </c>
-      <c r="G78" s="9">
-        <v>0.1437</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="D79" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E79" s="9">
-        <v>0.0966</v>
-      </c>
-      <c r="F79" s="9">
-        <v>0.1205</v>
-      </c>
-      <c r="G79" s="9">
-        <v>0.1063</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="C80" s="7">
-        <v>5.0E-5</v>
-      </c>
-      <c r="D80" s="3" t="s">
+      <c r="G81" s="3">
+        <v>0.2051</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="D82" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E80" s="3">
-        <v>0.1773</v>
-      </c>
-      <c r="F80" s="3">
-        <v>0.241</v>
-      </c>
-      <c r="G80" s="3">
-        <v>0.1766</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="D81" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E81" s="9">
-        <v>0.2103</v>
-      </c>
-      <c r="F81" s="9">
-        <v>0.1649</v>
-      </c>
-      <c r="G81" s="9">
-        <v>0.2051</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="D82" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E82" s="9">
+      <c r="E82" s="3">
         <v>0.1916</v>
       </c>
-      <c r="F82" s="9">
+      <c r="F82" s="3">
         <v>0.1734</v>
       </c>
-      <c r="G82" s="9">
+      <c r="G82" s="3">
         <v>0.1991</v>
       </c>
     </row>
     <row r="83">
-      <c r="D83" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E83" s="9">
+      <c r="D83" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E83" s="3">
         <v>0.2011</v>
       </c>
-      <c r="F83" s="9">
+      <c r="F83" s="3">
         <v>0.1839</v>
       </c>
-      <c r="G83" s="9">
+      <c r="G83" s="3">
         <v>0.1976</v>
       </c>
     </row>
     <row r="84">
-      <c r="C84" s="7">
+      <c r="C84" s="8">
         <v>1.0E-5</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D84" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="7">
+        <v>0.1594</v>
+      </c>
+      <c r="F84" s="7">
+        <v>0.1311</v>
+      </c>
+      <c r="G84" s="7">
+        <v>0.1243</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="D85" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E85" s="3">
+        <v>0.1097</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.1057</v>
+      </c>
+      <c r="G85" s="3">
+        <v>0.1198</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="D86" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E84" s="3">
-        <v>0.1594</v>
-      </c>
-      <c r="F84" s="3">
-        <v>0.1311</v>
-      </c>
-      <c r="G84" s="3">
-        <v>0.1243</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="D85" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E85" s="9">
-        <v>0.1097</v>
-      </c>
-      <c r="F85" s="9">
-        <v>0.1057</v>
-      </c>
-      <c r="G85" s="9">
-        <v>0.1198</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="D86" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E86" s="9">
+      <c r="E86" s="3">
         <v>0.1327</v>
       </c>
-      <c r="F86" s="9">
+      <c r="F86" s="3">
         <v>0.1755</v>
       </c>
-      <c r="G86" s="9">
+      <c r="G86" s="3">
         <v>0.1617</v>
       </c>
     </row>
     <row r="87">
-      <c r="D87" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E87" s="9">
+      <c r="D87" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E87" s="3">
         <v>0.104</v>
       </c>
-      <c r="F87" s="9">
+      <c r="F87" s="3">
         <v>0.1163</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="3">
         <v>0.11383</v>
       </c>
     </row>
     <row r="88">
-      <c r="C88" s="7">
+      <c r="C88" s="8">
         <v>1.0E-4</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E88" s="3">
+      <c r="D88" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E88" s="7">
         <v>0.2286</v>
       </c>
-      <c r="F88" s="3">
+      <c r="F88" s="7">
         <v>0.2579</v>
       </c>
-      <c r="G88" s="3">
+      <c r="G88" s="7">
         <v>0.2066</v>
       </c>
     </row>
     <row r="89">
       <c r="D89" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E89" s="3">
         <v>0.3012</v>
@@ -2302,7 +2434,7 @@
     </row>
     <row r="90">
       <c r="D90" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E90" s="3">
         <v>0.2067</v>
@@ -2316,7 +2448,7 @@
     </row>
     <row r="91">
       <c r="D91" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E91" s="3">
         <v>0.2159</v>
@@ -2329,25 +2461,25 @@
       </c>
     </row>
     <row r="92">
-      <c r="C92" s="7">
+      <c r="C92" s="8">
         <v>5.0E-4</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E92" s="3">
+      <c r="D92" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E92" s="7">
         <v>0.2131</v>
       </c>
-      <c r="F92" s="3">
+      <c r="F92" s="7">
         <v>0.1776</v>
       </c>
-      <c r="G92" s="3">
+      <c r="G92" s="7">
         <v>0.2051</v>
       </c>
     </row>
     <row r="93">
       <c r="D93" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E93" s="3">
         <v>0.2056</v>
@@ -2361,7 +2493,7 @@
     </row>
     <row r="94">
       <c r="D94" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E94" s="3">
         <v>0.2312</v>
@@ -2375,7 +2507,7 @@
     </row>
     <row r="95">
       <c r="D95" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E95" s="3">
         <v>0.2231</v>
@@ -2388,25 +2520,25 @@
       </c>
     </row>
     <row r="96">
-      <c r="C96" s="7">
+      <c r="C96" s="8">
         <v>0.001</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E96" s="3">
+      <c r="D96" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E96" s="7">
         <v>0.4155</v>
       </c>
-      <c r="F96" s="3">
+      <c r="F96" s="7">
         <v>0.1945</v>
       </c>
-      <c r="G96" s="3">
+      <c r="G96" s="7">
         <v>0.2021</v>
       </c>
     </row>
     <row r="97">
       <c r="D97" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E97" s="3">
         <v>0.2199</v>
@@ -2420,7 +2552,7 @@
     </row>
     <row r="98">
       <c r="D98" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E98" s="3">
         <v>0.2288</v>
@@ -2434,7 +2566,7 @@
     </row>
     <row r="99">
       <c r="D99" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E99" s="3">
         <v>0.2183</v>
@@ -2447,25 +2579,25 @@
       </c>
     </row>
     <row r="100">
-      <c r="C100" s="7">
+      <c r="C100" s="8">
         <v>0.005</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E100" s="3">
+      <c r="D100" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E100" s="7">
         <v>0.2107</v>
       </c>
-      <c r="F100" s="3">
+      <c r="F100" s="7">
         <v>0.1712</v>
       </c>
-      <c r="G100" s="3">
+      <c r="G100" s="7">
         <v>0.2081</v>
       </c>
     </row>
     <row r="101">
       <c r="D101" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E101" s="3">
         <v>0.2036</v>
@@ -2479,7 +2611,7 @@
     </row>
     <row r="102">
       <c r="D102" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E102" s="3">
         <v>0.2008</v>
@@ -2487,13 +2619,13 @@
       <c r="F102" s="3">
         <v>0.1712</v>
       </c>
-      <c r="G102" s="3">
+      <c r="G102" s="11">
         <v>0.2096</v>
       </c>
     </row>
     <row r="103">
       <c r="D103" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E103" s="3">
         <v>0.215</v>
@@ -2502,6 +2634,921 @@
         <v>0.1734</v>
       </c>
       <c r="G103" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="104" ht="40.5" customHeight="1">
+      <c r="A104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="C105" s="8">
+        <v>1.0E-4</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E105" s="7">
+        <v>0.2175</v>
+      </c>
+      <c r="F105" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="G105" s="7">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="D106" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" s="3">
+        <v>0.1977</v>
+      </c>
+      <c r="F106" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G106" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="D107" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E107" s="3">
+        <v>0.2159</v>
+      </c>
+      <c r="F107" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G107" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="D108" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E108" s="3">
+        <v>0.1738</v>
+      </c>
+      <c r="F108" s="3">
+        <v>0.1459</v>
+      </c>
+      <c r="G108" s="3">
+        <v>0.1302</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" s="8">
+        <v>0.001</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E109" s="7">
+        <v>0.2165</v>
+      </c>
+      <c r="F109" s="7">
+        <v>0.1712</v>
+      </c>
+      <c r="G109" s="7">
+        <v>0.2051</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="D110" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E110" s="3">
+        <v>0.2163</v>
+      </c>
+      <c r="F110" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G110" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="D111" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E111" s="3">
+        <v>0.2144</v>
+      </c>
+      <c r="F111" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G111" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="D112" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E112" s="3">
+        <v>0.2056</v>
+      </c>
+      <c r="F112" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G112" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="C113" s="8">
+        <v>0.005</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E113" s="7">
+        <v>0.2248</v>
+      </c>
+      <c r="F113" s="7">
+        <v>0.1712</v>
+      </c>
+      <c r="G113" s="7">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="D114" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E114" s="3">
+        <v>0.1204</v>
+      </c>
+      <c r="F114" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G114" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="D115" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E115" s="3">
+        <v>0.2056</v>
+      </c>
+      <c r="F115" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G115" s="11">
+        <v>0.2096</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="D116" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E116" s="3">
+        <v>0.2147</v>
+      </c>
+      <c r="F116" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G116" s="3">
+        <v>0.2096</v>
+      </c>
+    </row>
+    <row r="117" ht="38.25" customHeight="1">
+      <c r="A117" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="C118" s="8">
+        <v>1.0E-5</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E118" s="7">
+        <v>0.2105</v>
+      </c>
+      <c r="F118" s="7">
+        <v>0.186</v>
+      </c>
+      <c r="G118" s="7">
+        <v>0.1946</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="D119" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E119" s="3">
+        <v>0.1976</v>
+      </c>
+      <c r="F119" s="3">
+        <v>0.2452</v>
+      </c>
+      <c r="G119" s="3">
+        <v>0.1976</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="D120" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E120" s="3">
+        <v>0.2094</v>
+      </c>
+      <c r="F120" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G120" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="D121" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E121" s="3">
+        <v>0.2005</v>
+      </c>
+      <c r="F121" s="3">
+        <v>0.1755</v>
+      </c>
+      <c r="G121" s="3">
+        <v>0.1931</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="C122" s="8">
+        <v>1.0E-4</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E122" s="7">
+        <v>0.2157</v>
+      </c>
+      <c r="F122" s="7">
+        <v>0.1691</v>
+      </c>
+      <c r="G122" s="7">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="D123" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E123" s="3">
+        <v>0.214</v>
+      </c>
+      <c r="F123" s="3">
+        <v>0.2622</v>
+      </c>
+      <c r="G123" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="D124" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E124" s="3">
+        <v>0.2064</v>
+      </c>
+      <c r="F124" s="3">
+        <v>0.1734</v>
+      </c>
+      <c r="G124" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="D125" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E125" s="3">
+        <v>0.2344</v>
+      </c>
+      <c r="F125" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G125" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="C126" s="8">
+        <v>0.001</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E126" s="7">
+        <v>0.2366</v>
+      </c>
+      <c r="F126" s="7">
+        <v>0.1712</v>
+      </c>
+      <c r="G126" s="7">
+        <v>0.2051</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="D127" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E127" s="3">
+        <v>0.1972</v>
+      </c>
+      <c r="F127" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G127" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="D128" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E128" s="3">
+        <v>0.2141</v>
+      </c>
+      <c r="F128" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G128" s="3">
+        <v>0.2051</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="D129" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E129" s="3">
+        <v>0.2147</v>
+      </c>
+      <c r="F129" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G129" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="C130" s="8">
+        <v>0.005</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E130" s="7">
+        <v>0.2282</v>
+      </c>
+      <c r="F130" s="7">
+        <v>0.1712</v>
+      </c>
+      <c r="G130" s="11">
+        <v>0.2096</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="D131" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E131" s="3">
+        <v>0.2331</v>
+      </c>
+      <c r="F131" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G131" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="D132" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E132" s="3">
+        <v>0.2241</v>
+      </c>
+      <c r="F132" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G132" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="D133" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E133" s="3">
+        <v>0.2152</v>
+      </c>
+      <c r="F133" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G133" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="134" ht="36.0" customHeight="1">
+      <c r="A134" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D134" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="C135" s="8">
+        <v>1.0E-5</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E135" s="7">
+        <v>0.2167</v>
+      </c>
+      <c r="F135" s="7">
+        <v>0.1755</v>
+      </c>
+      <c r="G135" s="7">
+        <v>0.1976</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="D136" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E136" s="3">
+        <v>0.1984</v>
+      </c>
+      <c r="F136" s="3">
+        <v>0.1797</v>
+      </c>
+      <c r="G136" s="3">
+        <v>0.2051</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="D137" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E137" s="3">
+        <v>0.2066</v>
+      </c>
+      <c r="F137" s="3">
+        <v>0.2452</v>
+      </c>
+      <c r="G137" s="3">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="D138" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E138" s="3">
+        <v>0.1925</v>
+      </c>
+      <c r="F138" s="3">
+        <v>0.1649</v>
+      </c>
+      <c r="G138" s="3">
+        <v>0.2021</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="C139" s="8">
+        <v>1.0E-4</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E139" s="7">
+        <v>0.227</v>
+      </c>
+      <c r="F139" s="7">
+        <v>0.2622</v>
+      </c>
+      <c r="G139" s="7">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="D140" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E140" s="3">
+        <v>0.2244</v>
+      </c>
+      <c r="F140" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G140" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="D141" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E141" s="3">
+        <v>0.2163</v>
+      </c>
+      <c r="F141" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G141" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="D142" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E142" s="3">
+        <v>0.2238</v>
+      </c>
+      <c r="F142" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G142" s="3">
+        <v>0.2096</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="C143" s="8">
+        <v>0.001</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E143" s="7">
+        <v>0.219</v>
+      </c>
+      <c r="F143" s="7">
+        <v>0.1712</v>
+      </c>
+      <c r="G143" s="7">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="D144" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E144" s="3">
+        <v>0.2162</v>
+      </c>
+      <c r="F144" s="3">
+        <v>0.1691</v>
+      </c>
+      <c r="G144" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="D145" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E145" s="3">
+        <v>0.2222</v>
+      </c>
+      <c r="F145" s="3">
+        <v>0.167</v>
+      </c>
+      <c r="G145" s="14">
+        <v>0.2096</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D146" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="C147" s="15">
+        <v>1.0E-6</v>
+      </c>
+      <c r="D147" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E147" s="16">
+        <v>0.1067</v>
+      </c>
+      <c r="F147" s="16">
+        <v>0.1268</v>
+      </c>
+      <c r="G147" s="16">
+        <v>0.1168</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="D148" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E148" s="3">
+        <v>0.1268</v>
+      </c>
+      <c r="F148" s="3">
+        <v>0.1459</v>
+      </c>
+      <c r="G148" s="3">
+        <v>0.1692</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="D149" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E149" s="3">
+        <v>0.0922</v>
+      </c>
+      <c r="F149" s="3">
+        <v>0.1586</v>
+      </c>
+      <c r="G149" s="3">
+        <v>0.1123</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="D150" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E150" s="3">
+        <v>0.1443</v>
+      </c>
+      <c r="F150" s="3">
+        <v>0.13747</v>
+      </c>
+      <c r="G150" s="3">
+        <v>0.1422</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="D151" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E151" s="3">
+        <v>0.0898</v>
+      </c>
+      <c r="F151" s="3">
+        <v>0.0803</v>
+      </c>
+      <c r="G151" s="3">
+        <v>0.0689</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="C152" s="15">
+        <v>1.0E-5</v>
+      </c>
+      <c r="D152" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E152" s="16">
+        <v>0.206</v>
+      </c>
+      <c r="F152" s="16">
+        <v>0.1776</v>
+      </c>
+      <c r="G152" s="16">
+        <v>0.1991</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="D153" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E153" s="3">
+        <v>0.208</v>
+      </c>
+      <c r="F153" s="3">
+        <v>0.1628</v>
+      </c>
+      <c r="G153" s="3">
+        <v>0.2021</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="D154" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E154" s="3">
+        <v>0.1934</v>
+      </c>
+      <c r="F154" s="3">
+        <v>0.241</v>
+      </c>
+      <c r="G154" s="3">
+        <v>0.1991</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="D155" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E155" s="3">
+        <v>0.2127</v>
+      </c>
+      <c r="F155" s="3">
+        <v>0.1691</v>
+      </c>
+      <c r="G155" s="3">
+        <v>0.2051</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="D156" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E156" s="3">
+        <v>0.2075</v>
+      </c>
+      <c r="F156" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G156" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="C157" s="15">
+        <v>1.0E-4</v>
+      </c>
+      <c r="D157" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E157" s="16">
+        <v>0.2367</v>
+      </c>
+      <c r="F157" s="16">
+        <v>0.167</v>
+      </c>
+      <c r="G157" s="16">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="D158" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E158" s="3">
+        <v>0.1988</v>
+      </c>
+      <c r="F158" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G158" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="D159" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E159" s="3">
+        <v>0.2255</v>
+      </c>
+      <c r="F159" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G159" s="18">
+        <v>0.2111</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="D160" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E160" s="3">
+        <v>0.2108</v>
+      </c>
+      <c r="F160" s="3">
+        <v>0.2622</v>
+      </c>
+      <c r="G160" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="D161" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E161" s="3">
+        <v>0.2305</v>
+      </c>
+      <c r="F161" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G161" s="3">
+        <v>0.2096</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="C162" s="15">
+        <v>0.001</v>
+      </c>
+      <c r="D162" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E162" s="16">
+        <v>0.5869</v>
+      </c>
+      <c r="F162" s="16">
+        <v>0.1564</v>
+      </c>
+      <c r="G162" s="16">
+        <v>0.1722</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="D163" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E163" s="3">
+        <v>0.2234</v>
+      </c>
+      <c r="F163" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G163" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="D164" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E164" s="3">
+        <v>0.2235</v>
+      </c>
+      <c r="F164" s="3">
+        <v>0.1691</v>
+      </c>
+      <c r="G164" s="3">
+        <v>0.2066</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="D165" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E165" s="3">
+        <v>0.2208</v>
+      </c>
+      <c r="F165" s="3">
+        <v>0.1734</v>
+      </c>
+      <c r="G165" s="3">
+        <v>0.2081</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="D166" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E166" s="3">
+        <v>0.2115</v>
+      </c>
+      <c r="F166" s="3">
+        <v>0.1712</v>
+      </c>
+      <c r="G166" s="3">
         <v>0.2066</v>
       </c>
     </row>

</xml_diff>